<commit_message>
add comment in code and question 1 demo
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Repos\untitled\HKU_MFIN7002_Research_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E360172-9B33-463C-A3CA-23829AAA2BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BBFE7A-B793-4C29-B557-ADFBF3989EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="1140" windowWidth="20664" windowHeight="14616" activeTab="4" xr2:uid="{382386D0-A18B-4045-8BEA-4874332A251B}"/>
+    <workbookView xWindow="10944" yWindow="492" windowWidth="20664" windowHeight="14616" activeTab="1" xr2:uid="{382386D0-A18B-4045-8BEA-4874332A251B}"/>
   </bookViews>
   <sheets>
     <sheet name="Return Data" sheetId="2" r:id="rId1"/>
@@ -546,7 +546,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="53">
   <si>
     <t>Monthly Return Data</t>
   </si>
@@ -708,6 +708,18 @@
   </si>
   <si>
     <t>BTC absolute value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Developed-Market Equities Ex US</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emerging-Market Equities</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hedge Funds</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -13140,8 +13152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8818C3B-286B-46D7-A6D6-5B131D1064D7}">
   <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -16247,7 +16259,7 @@
   <dimension ref="A1:AJ68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -16305,13 +16317,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E2" s="78" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="G2" s="78" t="s">
         <v>8</v>
@@ -18707,7 +18719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D9AFCB-08B3-4194-A75D-D257FBCD3E96}">
   <dimension ref="A1:AJ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="87" workbookViewId="0">
       <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>

</xml_diff>